<commit_message>
Update done by teachers
</commit_message>
<xml_diff>
--- a/Grade 2018/MilestoneCompletion/Sem5_JSF_HBN_WS_Spring_Status.xlsx
+++ b/Grade 2018/MilestoneCompletion/Sem5_JSF_HBN_WS_Spring_Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\Sept 2020 - Jan 2021\Grade 2018\MilestoneCompletion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDCB294-6F12-4C8D-BC47-562F9222D869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1DA7A4-FAD2-4CDC-BC10-228917E7A289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="83">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -729,7 +729,7 @@
   <dimension ref="A1:AF60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
       <c r="D1" s="7"/>
       <c r="E1" s="6">
         <f ca="1">TODAY()</f>
-        <v>44095</v>
+        <v>44099</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1153,7 +1153,9 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
@@ -1176,7 +1178,9 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
@@ -1199,7 +1203,9 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1222,7 +1228,9 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1245,7 +1253,9 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1268,7 +1278,9 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="L19" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1291,7 +1303,9 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>